<commit_message>
#0 fill the table, modify the logic for duty of tests
</commit_message>
<xml_diff>
--- a/duties.xlsx
+++ b/duties.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28926"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB9B4D63-DF54-402B-BD0C-417A84B24F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{AB9B4D63-DF54-402B-BD0C-417A84B24F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610FEFDB-E828-43EF-9DAE-A95A650AD4FA}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4th Line" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
-  <si>
-    <t>Dmytro Latyshko</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="6">
   <si>
     <t>Pavlo Shtefan</t>
   </si>
   <si>
     <t>Olena Mikheyeva</t>
+  </si>
+  <si>
+    <t>Dmytro Latyshko</t>
   </si>
   <si>
     <t>Eugene Zinchenko</t>
@@ -395,7 +395,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -429,40 +429,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -472,36 +470,139 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
         <v>1</v>
       </c>
     </row>
@@ -517,15 +618,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7559BEA3B87EF459212D9B4B8BC4B83" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="020926a2805b8117b1690297fff31075">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69b2530c-d032-4638-9e6d-d03ad3bc3a8c" xmlns:ns3="24ccab74-1a8d-4d55-b2b6-44f573dd3e0c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7507ed44c30b3df59e2e18f8292da349" ns2:_="" ns3:_="">
     <xsd:import namespace="69b2530c-d032-4638-9e6d-d03ad3bc3a8c"/>
@@ -746,14 +838,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3933480-A8CD-4CDB-8F21-09AB85784D16}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BBB567B-CF54-4A60-9DAC-244AFD0A7428}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5FA8478-C49D-471B-86F7-6B09072E1665}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BBB567B-CF54-4A60-9DAC-244AFD0A7428}"/>
 </file>
</xml_diff>

<commit_message>
#0 add next nightly tests monitor, add retro responsible, reformat codes
</commit_message>
<xml_diff>
--- a/duties.xlsx
+++ b/duties.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{AB9B4D63-DF54-402B-BD0C-417A84B24F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610FEFDB-E828-43EF-9DAE-A95A650AD4FA}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{AB9B4D63-DF54-402B-BD0C-417A84B24F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41FBD23C-71B0-4C79-8829-E9E7DDD8B4E6}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4th Line" sheetId="1" r:id="rId1"/>
     <sheet name="Demo" sheetId="2" r:id="rId2"/>
     <sheet name="Night Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="Retro" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
   <si>
     <t>Pavlo Shtefan</t>
   </si>
@@ -51,6 +52,9 @@
   </si>
   <si>
     <t>Maria Donnik</t>
+  </si>
+  <si>
+    <t>Andrii Volkov</t>
   </si>
 </sst>
 </file>
@@ -394,9 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -472,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -611,10 +613,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C7A3A4-9B33-4BD1-96B1-6D3B7C1DD1FD}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -839,16 +897,13 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3933480-A8CD-4CDB-8F21-09AB85784D16}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5FA8478-C49D-471B-86F7-6B09072E1665}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -856,5 +911,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5FA8478-C49D-471B-86F7-6B09072E1665}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3933480-A8CD-4CDB-8F21-09AB85784D16}"/>
 </file>
</xml_diff>

<commit_message>
#0 add support json file, small refactoring, remove one duty person
</commit_message>
<xml_diff>
--- a/duties.xlsx
+++ b/duties.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29225"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{AB9B4D63-DF54-402B-BD0C-417A84B24F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41FBD23C-71B0-4C79-8829-E9E7DDD8B4E6}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{AB9B4D63-DF54-402B-BD0C-417A84B24F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E56DEF97-7CE6-4325-9CA7-B6CF9995217B}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4th Line" sheetId="1" r:id="rId1"/>
     <sheet name="Demo" sheetId="2" r:id="rId2"/>
-    <sheet name="Night Tests" sheetId="3" r:id="rId3"/>
-    <sheet name="Retro" sheetId="4" r:id="rId4"/>
+    <sheet name="Retro" sheetId="4" r:id="rId3"/>
+    <sheet name="Night Tests" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,18 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="6">
   <si>
-    <t>Pavlo Shtefan</t>
+    <t>Eugene Zinchenko</t>
   </si>
   <si>
     <t>Olena Mikheyeva</t>
   </si>
   <si>
     <t>Dmytro Latyshko</t>
-  </si>
-  <si>
-    <t>Eugene Zinchenko</t>
   </si>
   <si>
     <t>Andrii Vanikhin</t>
@@ -90,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,11 +394,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -417,213 +420,63 @@
         <v>2</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C7A3A4-9B33-4BD1-96B1-6D3B7C1DD1FD}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C7A3A4-9B33-4BD1-96B1-6D3B7C1DD1FD}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -638,7 +491,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -648,17 +501,12 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -666,13 +514,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -897,13 +860,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5FA8478-C49D-471B-86F7-6B09072E1665}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3933480-A8CD-4CDB-8F21-09AB85784D16}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -911,5 +877,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3933480-A8CD-4CDB-8F21-09AB85784D16}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5FA8478-C49D-471B-86F7-6B09072E1665}"/>
 </file>
</xml_diff>

<commit_message>
#0 fix duplicate duties of night tests duty
</commit_message>
<xml_diff>
--- a/duties.xlsx
+++ b/duties.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29227"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{AB9B4D63-DF54-402B-BD0C-417A84B24F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E56DEF97-7CE6-4325-9CA7-B6CF9995217B}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{AB9B4D63-DF54-402B-BD0C-417A84B24F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD775F39-6C35-4FBE-B10A-93F1E74B3ADF}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -516,10 +516,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection sqref="A1:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -544,86 +544,86 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -633,9 +633,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -860,16 +863,13 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3933480-A8CD-4CDB-8F21-09AB85784D16}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5FA8478-C49D-471B-86F7-6B09072E1665}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -877,5 +877,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5FA8478-C49D-471B-86F7-6B09072E1665}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3933480-A8CD-4CDB-8F21-09AB85784D16}"/>
 </file>
</xml_diff>